<commit_message>
Ajeitei o gráfico de artistas mais ouvidos
</commit_message>
<xml_diff>
--- a/Graficos/Grafico_Apps/data_apps_mais_usados.xlsx
+++ b/Graficos/Grafico_Apps/data_apps_mais_usados.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Usuários ativos por dia</t>
   </si>
   <si>
-    <t xml:space="preserve">Tempo de uso</t>
+    <t xml:space="preserve">Tempo de uso em segundos</t>
   </si>
   <si>
     <t xml:space="preserve">Tempo de uso médio</t>
@@ -140,7 +140,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -167,10 +167,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -197,15 +193,15 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="27"/>
   </cols>
   <sheetData>
@@ -273,7 +269,7 @@
       <c r="D4" s="6" t="n">
         <v>912</v>
       </c>
-      <c r="E4" s="8" t="n">
+      <c r="E4" s="7" t="n">
         <v>0.0105555555555556</v>
       </c>
     </row>

</xml_diff>